<commit_message>
test script that successfully changed my own pw 4 times automatically
</commit_message>
<xml_diff>
--- a/testSheet.xlsx
+++ b/testSheet.xlsx
@@ -25,16 +25,16 @@
     <t>Winter2024</t>
   </si>
   <si>
-    <t>Winter2023</t>
-  </si>
-  <si>
-    <t>1Winter2023</t>
-  </si>
-  <si>
-    <t>2Winter2023</t>
-  </si>
-  <si>
-    <t>3Winter2023</t>
+    <t>8Winter2023</t>
+  </si>
+  <si>
+    <t>9Winter2023</t>
+  </si>
+  <si>
+    <t>10Winter2023</t>
+  </si>
+  <si>
+    <t>11WInter2023</t>
   </si>
 </sst>
 </file>

</xml_diff>